<commit_message>
modified:   scripts/assets.ipynb 	modified:   scripts/my_portfolio.xlsx
</commit_message>
<xml_diff>
--- a/scripts/my_portfolio.xlsx
+++ b/scripts/my_portfolio.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -737,6 +737,117 @@
       <c r="I8" t="inlineStr">
         <is>
           <t>初始持仓</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-10-13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>卖出</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>海螺水泥</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" t="n">
+        <v>23.28</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2328</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2323</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>基本面不利</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-10-13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>卖出</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>立讯精密</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>62.32</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6232</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6227</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>止损</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-10-13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>卖出</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>华泰柏瑞中证红利低波动ETF链接A</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4126.61</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.6256</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6708.217215999999</v>
+      </c>
+      <c r="G11" t="n">
+        <v>33.54</v>
+      </c>
+      <c r="H11" t="n">
+        <v>6674.677215999999</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>止损</t>
         </is>
       </c>
     </row>
@@ -751,7 +862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -818,13 +929,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16000</v>
+        <v>31224.677216</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>16000</v>
+        <v>31224.677216</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -845,7 +956,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-13</t>
         </is>
       </c>
     </row>
@@ -856,13 +967,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16506.42</v>
+        <v>12379.81</v>
       </c>
       <c r="C3" t="n">
         <v>1.697010869565217</v>
       </c>
       <c r="D3" t="n">
-        <v>28011.57415760869</v>
+        <v>21008.67213315217</v>
       </c>
       <c r="E3" t="n">
         <v>1.6237</v>
@@ -883,7 +994,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-13</t>
         </is>
       </c>
     </row>
@@ -996,82 +1107,6 @@
         </is>
       </c>
       <c r="J6" t="inlineStr">
-        <is>
-          <t>2025-10-08</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>立讯精密</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>100</v>
-      </c>
-      <c r="C7" t="n">
-        <v>69.45458449645695</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6945.458449645695</v>
-      </c>
-      <c r="E7" t="n">
-        <v>64.69</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6469</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-476.4584496456946</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-6.86</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2025-10-08</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2025-10-08</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>海螺水泥</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>100</v>
-      </c>
-      <c r="C8" t="n">
-        <v>23.39075249320036</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2339.075249320036</v>
-      </c>
-      <c r="E8" t="n">
-        <v>23.22</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2322</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-17.07524932003616</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-0.73</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2025-10-08</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
         <is>
           <t>2025-10-08</t>
         </is>

</xml_diff>